<commit_message>
TText - adapted to SIAMv3
</commit_message>
<xml_diff>
--- a/TText/_IdP_TNO.xlsx
+++ b/TText/_IdP_TNO.xlsx
@@ -19,7 +19,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="J16" authorId="0">
+    <comment ref="J11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>Organization</t>
   </si>
@@ -122,9 +122,6 @@
     <t>[Role,]</t>
   </si>
   <si>
-    <t>Designer,User,Developer</t>
-  </si>
-  <si>
     <t>User,Developer</t>
   </si>
   <si>
@@ -137,12 +134,6 @@
     <t>TNO_P003</t>
   </si>
   <si>
-    <t>TNO_P004</t>
-  </si>
-  <si>
-    <t>TNO_P005</t>
-  </si>
-  <si>
     <t>Michiel</t>
   </si>
   <si>
@@ -161,45 +152,6 @@
     <t>Oosterheert</t>
   </si>
   <si>
-    <t>Silja</t>
-  </si>
-  <si>
-    <t>Eckhart</t>
-  </si>
-  <si>
-    <t>Jasper</t>
-  </si>
-  <si>
-    <t>Roes</t>
-  </si>
-  <si>
-    <t>TNO_P006</t>
-  </si>
-  <si>
-    <t>TNO_P007</t>
-  </si>
-  <si>
-    <t>Andre</t>
-  </si>
-  <si>
-    <t>Smulders</t>
-  </si>
-  <si>
-    <t>Jean-Louis</t>
-  </si>
-  <si>
-    <t>Roso</t>
-  </si>
-  <si>
-    <t>Johan</t>
-  </si>
-  <si>
-    <t>Ruiter</t>
-  </si>
-  <si>
-    <t>TNO_P008</t>
-  </si>
-  <si>
     <t>Acc_TNO_P001</t>
   </si>
   <si>
@@ -209,21 +161,6 @@
     <t>Acc_TNO_P003</t>
   </si>
   <si>
-    <t>Acc_TNO_P004</t>
-  </si>
-  <si>
-    <t>Acc_TNO_P005</t>
-  </si>
-  <si>
-    <t>Acc_TNO_P006</t>
-  </si>
-  <si>
-    <t>Acc_TNO_P007</t>
-  </si>
-  <si>
-    <t>Acc_TNO_P008</t>
-  </si>
-  <si>
     <t>AccountMgr,OrganizationMgr</t>
   </si>
   <si>
@@ -236,10 +173,10 @@
     <t>Acc_TNO_admin</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>autoLoginAccount</t>
+    <t>accAutoLoginReq</t>
+  </si>
+  <si>
+    <t>Designer,Developer</t>
   </si>
 </sst>
 </file>
@@ -629,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K13" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,351 +669,196 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="3" t="str">
+        <f>$A12</f>
+        <v>Account</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="B15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" t="str">
+        <f>$A15</f>
+        <v>Acc_TNO_P002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="3" t="str">
-        <f>$A17</f>
-        <v>Account</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="B16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J20" t="str">
-        <f>$A20</f>
-        <v>Acc_TNO_P002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>